<commit_message>
finish LC - 273
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henryxu/Desktop/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A85EB9-ED2A-A145-A3D1-ECA404DAA59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DC9A83-6563-774D-850C-83840C74140A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2563" uniqueCount="2528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="2529">
   <si>
     <t>Done</t>
   </si>
@@ -7626,6 +7626,9 @@
   </si>
   <si>
     <t>hashmap</t>
+  </si>
+  <si>
+    <t>math, string</t>
   </si>
 </sst>
 </file>
@@ -8857,8 +8860,8 @@
   <dimension ref="A1:O2501"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2197" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2236" sqref="F2236"/>
+      <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G274" sqref="G274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8928,7 +8931,7 @@
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>SUM(E2:E2501)</f>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -14410,10 +14413,16 @@
       <c r="C274" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D274" s="1"/>
-      <c r="E274" s="1"/>
-      <c r="F274" s="1"/>
-      <c r="G274" s="1"/>
+      <c r="D274" s="1" t="s">
+        <v>2528</v>
+      </c>
+      <c r="E274" s="1">
+        <v>1</v>
+      </c>
+      <c r="F274" s="12"/>
+      <c r="G274" s="1">
+        <v>1</v>
+      </c>
       <c r="H274" s="1"/>
       <c r="I274" s="1"/>
       <c r="J274" s="1"/>

</xml_diff>

<commit_message>
finish LC - 236
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henryxu/Desktop/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DC9A83-6563-774D-850C-83840C74140A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775216BD-1D17-AD4B-96FC-CFC68A26805A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="2529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2565" uniqueCount="2530">
   <si>
     <t>Done</t>
   </si>
@@ -7629,6 +7629,9 @@
   </si>
   <si>
     <t>math, string</t>
+  </si>
+  <si>
+    <t>tree, dfs, recursion</t>
   </si>
 </sst>
 </file>
@@ -7775,7 +7778,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8859,9 +8862,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2501"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G274" sqref="G274"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K237" sqref="K237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8931,7 +8934,7 @@
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>SUM(E2:E2501)</f>
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -13704,15 +13707,23 @@
       <c r="C237" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="D237" s="1"/>
-      <c r="E237" s="1"/>
-      <c r="F237" s="1"/>
+      <c r="D237" s="1" t="s">
+        <v>2529</v>
+      </c>
+      <c r="E237" s="1">
+        <v>1</v>
+      </c>
+      <c r="F237" s="12"/>
       <c r="G237" s="1"/>
       <c r="H237" s="1"/>
       <c r="I237" s="1"/>
       <c r="J237" s="1"/>
-      <c r="K237" s="1"/>
-      <c r="L237" s="1"/>
+      <c r="K237" s="1">
+        <v>1</v>
+      </c>
+      <c r="L237" s="1">
+        <v>1</v>
+      </c>
       <c r="M237" s="1"/>
       <c r="N237" s="1"/>
     </row>
@@ -14419,7 +14430,7 @@
       <c r="E274" s="1">
         <v>1</v>
       </c>
-      <c r="F274" s="12"/>
+      <c r="F274" s="6"/>
       <c r="G274" s="1">
         <v>1</v>
       </c>
@@ -51124,7 +51135,7 @@
       <c r="E2193" s="1">
         <v>1</v>
       </c>
-      <c r="F2193" s="12"/>
+      <c r="F2193" s="6"/>
       <c r="G2193" s="1">
         <v>1</v>
       </c>
@@ -51757,7 +51768,7 @@
       <c r="E2226" s="1">
         <v>1</v>
       </c>
-      <c r="F2226" s="12"/>
+      <c r="F2226" s="6"/>
       <c r="G2226" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
finish LC - 864
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henryxu/Desktop/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775216BD-1D17-AD4B-96FC-CFC68A26805A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C5C0B4-B938-A342-814C-4A26F8D4F540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2565" uniqueCount="2530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="2531">
   <si>
     <t>Done</t>
   </si>
@@ -7632,6 +7632,9 @@
   </si>
   <si>
     <t>tree, dfs, recursion</t>
+  </si>
+  <si>
+    <t>bfs, stateful visited set</t>
   </si>
 </sst>
 </file>
@@ -8862,9 +8865,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K237" sqref="K237"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A847" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F867" sqref="F867"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8934,7 +8937,7 @@
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>SUM(E2:E2501)</f>
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -25767,9 +25770,13 @@
       <c r="C865" s="1" t="s">
         <v>875</v>
       </c>
-      <c r="D865" s="1"/>
-      <c r="E865" s="1"/>
-      <c r="F865" s="1"/>
+      <c r="D865" s="1" t="s">
+        <v>2530</v>
+      </c>
+      <c r="E865" s="1">
+        <v>1</v>
+      </c>
+      <c r="F865" s="11"/>
       <c r="G865" s="1"/>
       <c r="H865" s="1"/>
       <c r="I865" s="1"/>
@@ -25777,7 +25784,9 @@
       <c r="K865" s="1"/>
       <c r="L865" s="1"/>
       <c r="M865" s="1"/>
-      <c r="N865" s="1"/>
+      <c r="N865" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="866" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B866" s="1">

</xml_diff>